<commit_message>
Update project with relevant changes
</commit_message>
<xml_diff>
--- a/test file.xlsx
+++ b/test file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asyrofifarel/Downloads/KILANG/Project_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAFAEEB-FA7B-614B-8033-EAC1E38BB0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ADE3F3-ECB6-1C44-A417-339856360420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{AD467CAF-8C7D-2D4E-8A26-9EF29153C8E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -83,9 +83,6 @@
     <t>volume_scaffolding</t>
   </si>
   <si>
-    <t>MA 2</t>
-  </si>
-  <si>
     <t>08 Januari 2025</t>
   </si>
   <si>
@@ -99,6 +96,33 @@
   </si>
   <si>
     <t>01 Januari 2025</t>
+  </si>
+  <si>
+    <t>tanggal_spk</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>UYE</t>
+  </si>
+  <si>
+    <t>12 Desember 2025</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>MA 4</t>
   </si>
 </sst>
 </file>
@@ -140,11 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8EC4B4-3E09-184B-A9AD-438F9F9DA9A4}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,9 +518,10 @@
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,8 +543,20 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -532,16 +570,28 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -555,20 +605,32 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D5" s="2"/>
     </row>
   </sheetData>

</xml_diff>